<commit_message>
Finished ANOVA and a high-fidelity linear regression for both 00 and 10 data, getting two distinct equations
</commit_message>
<xml_diff>
--- a/R/DP1_2010_20141114/multiple variable/Pearson Correlation_10.xlsx
+++ b/R/DP1_2010_20141114/multiple variable/Pearson Correlation_10.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jiaju\Documents\RData\DP1_2010_20141114\multiple variable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jiaju\Documents\RData\Final Project Data\ITWS-6350_DataScience\R\DP1_2010_20141114\multiple variable\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -58,7 +58,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -206,26 +206,26 @@
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,8 +515,8 @@
   <dimension ref="A2:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I8" sqref="I8"/>
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>